<commit_message>
Basics Requirements completed, scaling added.
</commit_message>
<xml_diff>
--- a/Match-Table-ID-Hand-wif-tests.xlsx
+++ b/Match-Table-ID-Hand-wif-tests.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Match Sheet " sheetId="1" r:id="rId1"/>
     <sheet name="Triplet Possibilities" sheetId="2" r:id="rId2"/>
     <sheet name="Pair Possibilities" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -636,9 +636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -914,9 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1236,9 +1232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>